<commit_message>
Diagramas de caso de uso adicionados
</commit_message>
<xml_diff>
--- a/Requisitos - João, Dienifer, Rodrigo, Gabriel F, Gabriel E.xlsx
+++ b/Requisitos - João, Dienifer, Rodrigo, Gabriel F, Gabriel E.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Ronaldo\Documents\GitHub\ana2017-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Ronaldo\Documents\Sistemas de Informação\9º semestre\ANA\Projetos\Diagramas de classe\RH\ana2017-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Requisito Funcionais" sheetId="2" r:id="rId1"/>
     <sheet name="Requisitos não Funcionais" sheetId="1" r:id="rId2"/>
     <sheet name="Requisitos de Dominio" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -100,12 +100,6 @@
     <t>RF003</t>
   </si>
   <si>
-    <t>Permitir avaliação dos motoristas, por parte dos usuários.</t>
-  </si>
-  <si>
-    <t>Permitir o bloqueio/denúncia de usuários/motoristas não capacitados para a Carona Solidária.</t>
-  </si>
-  <si>
     <t>Avaliação</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>RNF004</t>
   </si>
   <si>
-    <t>Bloqueio</t>
-  </si>
-  <si>
     <t>Usuário pode usar o App Jairo após se cadastrar</t>
   </si>
   <si>
@@ -182,12 +173,21 @@
   </si>
   <si>
     <t>Dienifer Belli Krauss</t>
+  </si>
+  <si>
+    <t>o usuário pode solicitar carona</t>
+  </si>
+  <si>
+    <t>Permitir avaliação dos motoristase e usuários, por ambas as partes do sistema.</t>
+  </si>
+  <si>
+    <t>Carona</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,38 +286,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -328,17 +307,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
@@ -651,9 +651,9 @@
       <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -664,7 +664,7 @@
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
@@ -677,7 +677,7 @@
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
@@ -705,156 +705,156 @@
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
+      <c r="B7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
@@ -870,333 +870,333 @@
       <c r="A24" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22" t="s">
+      <c r="F25" s="20"/>
+      <c r="G25" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21" t="s">
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22" t="s">
+      <c r="F26" s="20"/>
+      <c r="G26" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
+      <c r="B31" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21" t="s">
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22" t="s">
+      <c r="F32" s="20"/>
+      <c r="G32" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
+      <c r="B34" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
+      <c r="B38" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21" t="s">
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="21"/>
-      <c r="G39" s="22" t="s">
+      <c r="F39" s="20"/>
+      <c r="G39" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21" t="s">
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
+      <c r="B41" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
@@ -1211,69 +1211,69 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="23"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
@@ -1288,69 +1288,69 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
+      <c r="I60" s="27"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
+      <c r="A62" s="28"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
+      <c r="A63" s="28"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
+      <c r="A64" s="28"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
@@ -1365,69 +1365,69 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="9"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
+      <c r="I67" s="27"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="9"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="27"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
+      <c r="A69" s="28"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="23"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
+      <c r="A70" s="28"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
+      <c r="A71" s="28"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="23"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
@@ -1442,69 +1442,69 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="27"/>
+      <c r="I74" s="27"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="9"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="17"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="26"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="27"/>
+      <c r="I75" s="27"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
+      <c r="A76" s="28"/>
+      <c r="B76" s="23"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="13"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="14"/>
+      <c r="A77" s="28"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="23"/>
+      <c r="I77" s="23"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
-      <c r="B78" s="14"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
+      <c r="A78" s="28"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="23"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
@@ -1519,69 +1519,69 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="23"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="9"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="16"/>
-      <c r="F81" s="16"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="27"/>
+      <c r="I81" s="27"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
-      <c r="B82" s="14"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="16"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+      <c r="G82" s="27"/>
+      <c r="H82" s="27"/>
+      <c r="I82" s="27"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
-      <c r="B83" s="14"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14"/>
+      <c r="A83" s="28"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="23"/>
+      <c r="I83" s="23"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
+      <c r="A84" s="28"/>
+      <c r="B84" s="23"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
+      <c r="H84" s="23"/>
+      <c r="I84" s="23"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="13"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
+      <c r="A85" s="28"/>
+      <c r="B85" s="23"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
+      <c r="H85" s="23"/>
+      <c r="I85" s="23"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
@@ -1596,69 +1596,69 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
+      <c r="H87" s="23"/>
+      <c r="I87" s="23"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="9"/>
-      <c r="B88" s="14"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="16"/>
-      <c r="F88" s="16"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-      <c r="I88" s="17"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="27"/>
+      <c r="H88" s="27"/>
+      <c r="I88" s="27"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="9"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="16"/>
-      <c r="F89" s="16"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
+      <c r="B89" s="23"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="26"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="27"/>
+      <c r="I89" s="27"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="13"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
+      <c r="A90" s="28"/>
+      <c r="B90" s="23"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="23"/>
+      <c r="I90" s="23"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="13"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="14"/>
+      <c r="A91" s="28"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
+      <c r="H91" s="23"/>
+      <c r="I91" s="23"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="13"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="14"/>
+      <c r="A92" s="28"/>
+      <c r="B92" s="23"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
+      <c r="H92" s="23"/>
+      <c r="I92" s="23"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
@@ -1673,90 +1673,6 @@
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:I20"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:I29"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:I36"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:I43"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="B59:I59"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:I50"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:I57"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="G61:I61"/>
-    <mergeCell ref="B73:I73"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B62:I64"/>
-    <mergeCell ref="B66:I66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:I71"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="G75:I75"/>
-    <mergeCell ref="B76:I78"/>
-    <mergeCell ref="B80:I80"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="G81:I81"/>
     <mergeCell ref="A90:A92"/>
     <mergeCell ref="B90:I92"/>
     <mergeCell ref="B5:I5"/>
@@ -1773,6 +1689,90 @@
     <mergeCell ref="B83:I85"/>
     <mergeCell ref="B87:I87"/>
     <mergeCell ref="A76:A78"/>
+    <mergeCell ref="B76:I78"/>
+    <mergeCell ref="B80:I80"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="G81:I81"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="G75:I75"/>
+    <mergeCell ref="B73:I73"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B62:I64"/>
+    <mergeCell ref="B66:I66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:I71"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="B59:I59"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:I50"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:I57"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:I36"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:I43"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:I20"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:I29"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1794,7 +1794,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
@@ -1809,7 +1809,7 @@
       <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="15" t="str">
         <f>'Requisito Funcionais'!B2:I2</f>
         <v>Dienifer Belli Krauss</v>
@@ -1823,7 +1823,7 @@
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
@@ -1836,7 +1836,7 @@
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
@@ -1864,19 +1864,19 @@
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
+      <c r="B7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="31" t="str">
@@ -1892,7 +1892,7 @@
       <c r="I9" s="31"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
       <c r="D10" s="31"/>
@@ -1903,7 +1903,7 @@
       <c r="I10" s="31"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
@@ -2004,17 +2004,17 @@
       <c r="I20" s="31"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
@@ -2028,331 +2028,331 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+        <v>34</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
+      <c r="B27" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
+        <v>35</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
+      <c r="B34" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21" t="s">
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="21"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21" t="s">
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
+      <c r="B41" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
+        <v>37</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21" t="s">
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F46" s="21"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="21" t="s">
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F47" s="21"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="22"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29"/>
-      <c r="I48" s="29"/>
+      <c r="B48" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="29"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
@@ -2732,14 +2732,33 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:I50"/>
+    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:I43"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:I36"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:I33"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="B27:I29"/>
@@ -2751,33 +2770,14 @@
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B9:I20"/>
     <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:I36"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:I43"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:I50"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2799,7 +2799,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
@@ -2814,7 +2814,7 @@
       <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="15" t="str">
         <f>'Requisito Funcionais'!B2:I2</f>
         <v>Dienifer Belli Krauss</v>
@@ -2828,7 +2828,7 @@
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
@@ -2841,7 +2841,7 @@
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
@@ -2869,19 +2869,19 @@
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
+      <c r="B7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="31" t="str">
@@ -2897,7 +2897,7 @@
       <c r="I9" s="31"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
       <c r="D10" s="31"/>
@@ -2908,7 +2908,7 @@
       <c r="I10" s="31"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
@@ -3009,17 +3009,17 @@
       <c r="I20" s="31"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
@@ -3033,249 +3033,249 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+        <v>40</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="B27" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
+        <v>41</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
+      <c r="B34" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21" t="s">
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="21"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21" t="s">
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
+      <c r="B41" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
@@ -3884,6 +3884,29 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:I43"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:I36"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B27:I29"/>
     <mergeCell ref="B5:I5"/>
@@ -3897,30 +3920,7 @@
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
     <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:I36"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:I43"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>